<commit_message>
fix identifier & tests
</commit_message>
<xml_diff>
--- a/test/fixtures/files/customer_sales_test.xlsx
+++ b/test/fixtures/files/customer_sales_test.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Tuote/Asiakas</t>
+    <t>Asiakas/Tuote</t>
   </si>
   <si>
     <t>Kpl</t>
@@ -55,6 +55,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,12 +140,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.1479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>